<commit_message>
idk - almost finish - not working.
</commit_message>
<xml_diff>
--- a/letters.xlsx
+++ b/letters.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="List2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="85">
   <si>
     <t>A</t>
   </si>
@@ -160,6 +161,120 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>celkové skóre</t>
+  </si>
+  <si>
+    <t>trojice [%]</t>
+  </si>
+  <si>
+    <t>dvojice [%]</t>
+  </si>
+  <si>
+    <t>dvojice stejných písmen [%]</t>
+  </si>
+  <si>
+    <t>jednopísmenová slova [%]</t>
+  </si>
+  <si>
+    <t>na konci slov [%]</t>
+  </si>
+  <si>
+    <t>na začátku slov [%]</t>
+  </si>
+  <si>
+    <t>v celém textu [%]</t>
+  </si>
+  <si>
+    <t>písmeno</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>Klíč</t>
+  </si>
+  <si>
+    <t>Uhádnutý klíč</t>
+  </si>
+  <si>
+    <t>1.</t>
   </si>
 </sst>
 </file>
@@ -187,15 +302,57 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -248,11 +405,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -276,6 +593,88 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -558,21 +957,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M52"/>
+  <dimension ref="B1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J28"/>
+    <sheetView topLeftCell="B51" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="29.85546875" customWidth="1"/>
     <col min="12" max="12" width="16.5703125" customWidth="1"/>
     <col min="13" max="13" width="34.28515625" customWidth="1"/>
@@ -636,7 +1035,7 @@
         <v>8.5072231139646899</v>
       </c>
       <c r="J3" s="3">
-        <f>C3+D3+E3+F3*10+G3+H3*2+I3*3</f>
+        <f t="shared" ref="J3:J28" si="0">C3+D3+E3+F3*10+G3+H3*2+I3*3</f>
         <v>826.63892411896404</v>
       </c>
       <c r="L3" s="2">
@@ -668,7 +1067,7 @@
         <v>6.0995184590690199</v>
       </c>
       <c r="J4" s="3">
-        <f>C4+D4+E4+F4*10+G4+H4*2+I4*3</f>
+        <f t="shared" si="0"/>
         <v>301.32895028166564</v>
       </c>
       <c r="L4" s="2"/>
@@ -698,7 +1097,7 @@
         <v>18.726591760299623</v>
       </c>
       <c r="J5" s="3">
-        <f>C5+D5+E5+F5*10+G5+H5*2+I5*3</f>
+        <f t="shared" si="0"/>
         <v>130.68212527550105</v>
       </c>
       <c r="L5" s="2"/>
@@ -726,7 +1125,7 @@
         <v>18.726591760299623</v>
       </c>
       <c r="J6" s="3">
-        <f>C6+D6+E6+F6*10+G6+H6*2+I6*3</f>
+        <f t="shared" si="0"/>
         <v>123.92073037104245</v>
       </c>
       <c r="L6" s="2">
@@ -756,7 +1155,7 @@
         <v>18.726591760299623</v>
       </c>
       <c r="J7" s="3">
-        <f>C7+D7+E7+F7*10+G7+H7*2+I7*3</f>
+        <f t="shared" si="0"/>
         <v>101.09813196879696</v>
       </c>
       <c r="L7" s="2">
@@ -788,7 +1187,7 @@
         <v>14.606741573033707</v>
       </c>
       <c r="J8" s="3">
-        <f>C8+D8+E8+F8*10+G8+H8*2+I8*3</f>
+        <f t="shared" si="0"/>
         <v>87.609511343304945</v>
       </c>
       <c r="L8" s="2"/>
@@ -816,7 +1215,7 @@
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="3">
-        <f>C9+D9+E9+F9*10+G9+H9*2+I9*3</f>
+        <f t="shared" si="0"/>
         <v>60.830251106552957</v>
       </c>
       <c r="L9" s="2">
@@ -848,7 +1247,7 @@
         <v>8.5072231139646863</v>
       </c>
       <c r="J10" s="3">
-        <f>C10+D10+E10+F10*10+G10+H10*2+I10*3</f>
+        <f t="shared" si="0"/>
         <v>50.719255329155203</v>
       </c>
       <c r="L10" s="2">
@@ -880,7 +1279,7 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="3">
-        <f>C11+D11+E11+F11*10+G11+H11*2+I11*3</f>
+        <f t="shared" si="0"/>
         <v>42.839143150167338</v>
       </c>
       <c r="L11" s="2">
@@ -910,7 +1309,7 @@
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="3">
-        <f>C12+D12+E12+F12*10+G12+H12*2+I12*3</f>
+        <f t="shared" si="0"/>
         <v>30.684649681528661</v>
       </c>
       <c r="L12" s="2"/>
@@ -936,7 +1335,7 @@
         <v>6.0995184590690199</v>
       </c>
       <c r="J13" s="3">
-        <f>C13+D13+E13+F13*10+G13+H13*2+I13*3</f>
+        <f t="shared" si="0"/>
         <v>25.607504421793045</v>
       </c>
       <c r="L13" s="2"/>
@@ -962,7 +1361,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="3">
-        <f>C14+D14+E14+F14*10+G14+H14*2+I14*3</f>
+        <f t="shared" si="0"/>
         <v>23.154406779661016</v>
       </c>
       <c r="L14" s="2"/>
@@ -988,7 +1387,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="3">
-        <f>C15+D15+E15+F15*10+G15+H15*2+I15*3</f>
+        <f t="shared" si="0"/>
         <v>21.951406779661017</v>
       </c>
       <c r="L15" s="2"/>
@@ -1012,7 +1411,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="3">
-        <f>C16+D16+E16+F16*10+G16+H16*2+I16*3</f>
+        <f t="shared" si="0"/>
         <v>15.263576271186441</v>
       </c>
       <c r="L16" s="2" t="s">
@@ -1040,7 +1439,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="3">
-        <f>C17+D17+E17+F17*10+G17+H17*2+I17*3</f>
+        <f t="shared" si="0"/>
         <v>11.247999999999999</v>
       </c>
       <c r="L17" s="2"/>
@@ -1064,7 +1463,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3">
-        <f>C18+D18+E18+F18*10+G18+H18*2+I18*3</f>
+        <f t="shared" si="0"/>
         <v>9.1129999999999995</v>
       </c>
       <c r="L18" s="2"/>
@@ -1088,7 +1487,7 @@
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3">
-        <f>C19+D19+E19+F19*10+G19+H19*2+I19*3</f>
+        <f t="shared" si="0"/>
         <v>8.3214331210191084</v>
       </c>
       <c r="L19" s="2"/>
@@ -1110,7 +1509,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3">
-        <f>C20+D20+E20+F20*10+G20+H20*2+I20*3</f>
+        <f t="shared" si="0"/>
         <v>6.2930000000000001</v>
       </c>
       <c r="L20" s="2"/>
@@ -1134,7 +1533,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3">
-        <f>C21+D21+E21+F21*10+G21+H21*2+I21*3</f>
+        <f t="shared" si="0"/>
         <v>6.194</v>
       </c>
       <c r="L21" s="2"/>
@@ -1158,7 +1557,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3">
-        <f>C22+D22+E22+F22*10+G22+H22*2+I22*3</f>
+        <f t="shared" si="0"/>
         <v>4.4740000000000002</v>
       </c>
       <c r="L22" s="2">
@@ -1184,7 +1583,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3">
-        <f>C23+D23+E23+F23*10+G23+H23*2+I23*3</f>
+        <f t="shared" si="0"/>
         <v>1.627</v>
       </c>
       <c r="L23" s="2"/>
@@ -1208,7 +1607,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3">
-        <f>C24+D24+E24+F24*10+G24+H24*2+I24*3</f>
+        <f t="shared" si="0"/>
         <v>1.3620000000000001</v>
       </c>
       <c r="K24" s="3"/>
@@ -1230,7 +1629,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3">
-        <f>C25+D25+E25+F25*10+G25+H25*2+I25*3</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
       <c r="K25" s="3"/>
@@ -1252,7 +1651,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3">
-        <f>C26+D26+E26+F26*10+G26+H26*2+I26*3</f>
+        <f t="shared" si="0"/>
         <v>0.26800000000000002</v>
       </c>
       <c r="K26" s="3"/>
@@ -1274,7 +1673,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3">
-        <f>C27+D27+E27+F27*10+G27+H27*2+I27*3</f>
+        <f t="shared" si="0"/>
         <v>0.16699999999999998</v>
       </c>
       <c r="K27" s="3"/>
@@ -1296,7 +1695,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3">
-        <f>C28+D28+E28+F28*10+G28+H28*2+I28*3</f>
+        <f t="shared" si="0"/>
         <v>0.108</v>
       </c>
       <c r="K28" s="2"/>
@@ -1336,21 +1735,21 @@
         <v>10</v>
       </c>
       <c r="G34">
-        <f t="shared" ref="G34:G43" si="0">100*F34/$F$44</f>
+        <f t="shared" ref="G34:G43" si="1">100*F34/$F$44</f>
         <v>16.949152542372882</v>
       </c>
       <c r="H34" s="3">
         <v>5.6</v>
       </c>
       <c r="I34">
-        <f t="shared" ref="I34:I49" si="1">H34*100/$H$52</f>
+        <f t="shared" ref="I34:I49" si="2">H34*100/$H$52</f>
         <v>8.9171974522292992</v>
       </c>
       <c r="K34" s="3">
         <v>1.1399999999999999</v>
       </c>
       <c r="L34">
-        <f t="shared" ref="L34:L47" si="2">100*K34/$K$49</f>
+        <f t="shared" ref="L34:L47" si="3">100*K34/$K$49</f>
         <v>6.0995184590690199</v>
       </c>
     </row>
@@ -1359,61 +1758,61 @@
         <v>15</v>
       </c>
       <c r="G35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.423728813559322</v>
       </c>
       <c r="H35" s="3">
         <v>7.51</v>
       </c>
       <c r="I35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11.95859872611465</v>
       </c>
       <c r="K35" s="3">
         <v>3.5</v>
       </c>
       <c r="L35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.726591760299623</v>
       </c>
     </row>
     <row r="36" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F36" s="3"/>
       <c r="G36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H36" s="3">
         <v>11.33</v>
       </c>
       <c r="I36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.041401273885352</v>
       </c>
       <c r="K36" s="3">
         <v>3.5</v>
       </c>
       <c r="L36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.726591760299623</v>
       </c>
     </row>
     <row r="37" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F37" s="3"/>
       <c r="G37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H37" s="3">
         <v>2.19</v>
       </c>
       <c r="I37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4872611464968153</v>
       </c>
       <c r="K37" s="3"/>
       <c r="L37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1422,61 +1821,61 @@
         <v>5</v>
       </c>
       <c r="G38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.4745762711864412</v>
       </c>
       <c r="H38" s="3">
         <v>9.92</v>
       </c>
       <c r="I38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.796178343949045</v>
       </c>
       <c r="K38" s="3">
         <v>3.5</v>
       </c>
       <c r="L38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.726591760299623</v>
       </c>
     </row>
     <row r="39" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F39" s="3"/>
       <c r="G39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H39" s="3">
         <v>8.42</v>
       </c>
       <c r="I39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.407643312101911</v>
       </c>
       <c r="K39" s="3">
         <v>2.73</v>
       </c>
       <c r="L39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14.606741573033707</v>
       </c>
     </row>
     <row r="40" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F40" s="3"/>
       <c r="G40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H40" s="3">
         <v>5</v>
       </c>
       <c r="I40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.9617834394904463</v>
       </c>
       <c r="K40" s="3"/>
       <c r="L40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1485,21 +1884,21 @@
         <v>7</v>
       </c>
       <c r="G41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.864406779661017</v>
       </c>
       <c r="H41" s="3">
         <v>2.84</v>
       </c>
       <c r="I41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.5222929936305736</v>
       </c>
       <c r="K41" s="3">
         <v>1.59</v>
       </c>
       <c r="L41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.5072231139646863</v>
       </c>
     </row>
@@ -1508,19 +1907,19 @@
         <v>7</v>
       </c>
       <c r="G42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.864406779661017</v>
       </c>
       <c r="H42" s="3">
         <v>5.0599999999999996</v>
       </c>
       <c r="I42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.0573248407643305</v>
       </c>
       <c r="K42" s="3"/>
       <c r="L42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1529,17 +1928,17 @@
         <v>5</v>
       </c>
       <c r="G43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.4745762711864412</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K43" s="3"/>
       <c r="L43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1550,36 +1949,36 @@
       </c>
       <c r="H44" s="3"/>
       <c r="I44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K44" s="3"/>
       <c r="L44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H45" s="3"/>
       <c r="I45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K45" s="3"/>
       <c r="L45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H46" s="3"/>
       <c r="I46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K46" s="3"/>
       <c r="L46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1588,30 +1987,30 @@
         <v>1.05</v>
       </c>
       <c r="I47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6719745222929938</v>
       </c>
       <c r="K47" s="3">
         <v>1.1399999999999999</v>
       </c>
       <c r="L47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.0995184590690199</v>
       </c>
     </row>
     <row r="48" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H48" s="3"/>
       <c r="I48">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="8:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H49" s="3">
         <v>1.28</v>
       </c>
       <c r="I49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0382165605095541</v>
       </c>
       <c r="K49">
@@ -1619,23 +2018,1441 @@
         <v>18.690000000000001</v>
       </c>
     </row>
-    <row r="50" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H52" s="3">
         <f>SUM(H33:H49)</f>
         <v>62.8</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G57" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H57" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I57" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J57" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="L57">
+        <f>26-2-4-5</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="24"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="20"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B59" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="16">
+        <v>8.1669999999999998</v>
+      </c>
+      <c r="D59" s="16">
+        <v>15.5</v>
+      </c>
+      <c r="E59" s="16">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="F59" s="16">
+        <v>75</v>
+      </c>
+      <c r="G59" s="16">
+        <v>0</v>
+      </c>
+      <c r="H59" s="16">
+        <v>4.1401273885350323</v>
+      </c>
+      <c r="I59" s="16">
+        <v>8.5072231139646899</v>
+      </c>
+      <c r="J59" s="16">
+        <f t="shared" ref="J59:J84" si="4">C59+D59+E59+F59*10+G59+H59*2+I59*3</f>
+        <v>826.63892411896404</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="10">
+        <v>6.9660000000000002</v>
+      </c>
+      <c r="D60" s="10">
+        <v>8.23</v>
+      </c>
+      <c r="E60" s="10">
+        <v>0</v>
+      </c>
+      <c r="F60" s="10">
+        <v>25</v>
+      </c>
+      <c r="G60" s="10">
+        <v>0</v>
+      </c>
+      <c r="H60" s="10">
+        <v>8.9171974522292992</v>
+      </c>
+      <c r="I60" s="10">
+        <v>6.0995184590690199</v>
+      </c>
+      <c r="J60" s="10">
+        <f t="shared" si="4"/>
+        <v>301.32895028166564</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B61" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="16">
+        <v>9.0559999999999992</v>
+      </c>
+      <c r="D61" s="16">
+        <v>15.94</v>
+      </c>
+      <c r="E61" s="16">
+        <v>8.64</v>
+      </c>
+      <c r="F61" s="16">
+        <v>0</v>
+      </c>
+      <c r="G61" s="16">
+        <v>16.949152542372882</v>
+      </c>
+      <c r="H61" s="16">
+        <v>11.95859872611465</v>
+      </c>
+      <c r="I61" s="16">
+        <v>18.726591760299623</v>
+      </c>
+      <c r="J61" s="16">
+        <f t="shared" si="4"/>
+        <v>130.68212527550105</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B62" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="10">
+        <v>12.702</v>
+      </c>
+      <c r="D62" s="10">
+        <v>2.0070000000000001</v>
+      </c>
+      <c r="E62" s="10">
+        <v>0</v>
+      </c>
+      <c r="F62" s="10">
+        <v>0</v>
+      </c>
+      <c r="G62" s="10">
+        <v>16.949152542372882</v>
+      </c>
+      <c r="H62" s="10">
+        <v>18.041401273885352</v>
+      </c>
+      <c r="I62" s="10">
+        <v>18.726591760299623</v>
+      </c>
+      <c r="J62" s="10">
+        <f t="shared" si="4"/>
+        <v>123.92073037104245</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B63" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="16">
+        <v>6.0940000000000003</v>
+      </c>
+      <c r="D63" s="16">
+        <v>7.2320000000000002</v>
+      </c>
+      <c r="E63" s="16">
+        <v>0</v>
+      </c>
+      <c r="F63" s="16">
+        <v>0</v>
+      </c>
+      <c r="G63" s="16">
+        <v>0</v>
+      </c>
+      <c r="H63" s="16">
+        <v>15.796178343949045</v>
+      </c>
+      <c r="I63" s="16">
+        <v>18.726591760299623</v>
+      </c>
+      <c r="J63" s="16">
+        <f t="shared" si="4"/>
+        <v>101.09813196879696</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B64" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="14">
+        <v>6.7489999999999997</v>
+      </c>
+      <c r="D64" s="14">
+        <v>2.3650000000000002</v>
+      </c>
+      <c r="E64" s="14">
+        <v>7.86</v>
+      </c>
+      <c r="F64" s="14">
+        <v>0</v>
+      </c>
+      <c r="G64" s="14">
+        <v>0</v>
+      </c>
+      <c r="H64" s="14">
+        <v>13.407643312101911</v>
+      </c>
+      <c r="I64" s="14">
+        <v>14.606741573033707</v>
+      </c>
+      <c r="J64" s="14">
+        <f t="shared" si="4"/>
+        <v>87.609511343304945</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="16">
+        <v>6.327</v>
+      </c>
+      <c r="D65" s="16">
+        <v>7.7549999999999999</v>
+      </c>
+      <c r="E65" s="16">
+        <v>14.35</v>
+      </c>
+      <c r="F65" s="16">
+        <v>0</v>
+      </c>
+      <c r="G65" s="16">
+        <v>25.4237288135593</v>
+      </c>
+      <c r="H65" s="16">
+        <v>3.4872611464968153</v>
+      </c>
+      <c r="I65" s="16">
+        <v>0</v>
+      </c>
+      <c r="J65" s="16">
+        <f t="shared" si="4"/>
+        <v>60.830251106552936</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="12">
+        <v>4.2530000000000001</v>
+      </c>
+      <c r="D66" s="12">
+        <v>2.67</v>
+      </c>
+      <c r="E66" s="12">
+        <v>9.23</v>
+      </c>
+      <c r="F66" s="12">
+        <v>0</v>
+      </c>
+      <c r="G66" s="12">
+        <v>0</v>
+      </c>
+      <c r="H66" s="12">
+        <v>4.5222929936305736</v>
+      </c>
+      <c r="I66" s="12">
+        <v>8.5072231139646899</v>
+      </c>
+      <c r="J66" s="12">
+        <f t="shared" si="4"/>
+        <v>50.719255329155217</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="16">
+        <v>7.5069999999999997</v>
+      </c>
+      <c r="D67" s="16">
+        <v>6.2640000000000002</v>
+      </c>
+      <c r="E67" s="16">
+        <v>4.67</v>
+      </c>
+      <c r="F67" s="16">
+        <v>0</v>
+      </c>
+      <c r="G67" s="16">
+        <v>8.4745762711864412</v>
+      </c>
+      <c r="H67" s="16">
+        <v>7.9617834394904463</v>
+      </c>
+      <c r="I67" s="16">
+        <v>0</v>
+      </c>
+      <c r="J67" s="16">
+        <f t="shared" si="4"/>
+        <v>42.839143150167338</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="10">
+        <v>5.9870000000000001</v>
+      </c>
+      <c r="D68" s="10">
+        <v>1.653</v>
+      </c>
+      <c r="E68" s="10">
+        <v>6.93</v>
+      </c>
+      <c r="F68" s="10">
+        <v>0</v>
+      </c>
+      <c r="G68" s="10">
+        <v>0</v>
+      </c>
+      <c r="H68" s="10">
+        <v>8.0573248407643305</v>
+      </c>
+      <c r="I68" s="10">
+        <v>0</v>
+      </c>
+      <c r="J68" s="10">
+        <f t="shared" si="4"/>
+        <v>30.684649681528661</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="16">
+        <v>2.0150000000000001</v>
+      </c>
+      <c r="D69" s="16">
+        <v>1.95</v>
+      </c>
+      <c r="E69" s="16">
+        <v>0</v>
+      </c>
+      <c r="F69" s="16">
+        <v>0</v>
+      </c>
+      <c r="G69" s="16">
+        <v>0</v>
+      </c>
+      <c r="H69" s="16">
+        <v>1.6719745222929938</v>
+      </c>
+      <c r="I69" s="16">
+        <v>6.0995184590690199</v>
+      </c>
+      <c r="J69" s="16">
+        <f t="shared" si="4"/>
+        <v>25.607504421793045</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="10">
+        <v>4.0250000000000004</v>
+      </c>
+      <c r="D70" s="10">
+        <v>2.7050000000000001</v>
+      </c>
+      <c r="E70" s="10">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="F70" s="10">
+        <v>0</v>
+      </c>
+      <c r="G70" s="10">
+        <v>11.864406779661017</v>
+      </c>
+      <c r="H70" s="10">
+        <v>0</v>
+      </c>
+      <c r="I70" s="10">
+        <v>0</v>
+      </c>
+      <c r="J70" s="10">
+        <f t="shared" si="4"/>
+        <v>23.154406779661016</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="16">
+        <v>2.2280000000000002</v>
+      </c>
+      <c r="D71" s="16">
+        <v>3.7789999999999999</v>
+      </c>
+      <c r="E71" s="16">
+        <v>4.08</v>
+      </c>
+      <c r="F71" s="16">
+        <v>0</v>
+      </c>
+      <c r="G71" s="16">
+        <v>11.864406779661017</v>
+      </c>
+      <c r="H71" s="16">
+        <v>0</v>
+      </c>
+      <c r="I71" s="16">
+        <v>0</v>
+      </c>
+      <c r="J71" s="16">
+        <f t="shared" si="4"/>
+        <v>21.951406779661017</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72" s="10">
+        <v>2.4060000000000001</v>
+      </c>
+      <c r="D72" s="10">
+        <v>4.383</v>
+      </c>
+      <c r="E72" s="10">
+        <v>0</v>
+      </c>
+      <c r="F72" s="10">
+        <v>0</v>
+      </c>
+      <c r="G72" s="10">
+        <v>8.4745762711864412</v>
+      </c>
+      <c r="H72" s="10">
+        <v>0</v>
+      </c>
+      <c r="I72" s="10">
+        <v>0</v>
+      </c>
+      <c r="J72" s="10">
+        <f t="shared" si="4"/>
+        <v>15.263576271186441</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" s="16">
+        <v>1.974</v>
+      </c>
+      <c r="D73" s="16">
+        <v>1.974</v>
+      </c>
+      <c r="E73" s="16">
+        <v>7.3</v>
+      </c>
+      <c r="F73" s="16">
+        <v>0</v>
+      </c>
+      <c r="G73" s="16">
+        <v>0</v>
+      </c>
+      <c r="H73" s="16">
+        <v>0</v>
+      </c>
+      <c r="I73" s="16">
+        <v>0</v>
+      </c>
+      <c r="J73" s="16">
+        <f t="shared" si="4"/>
+        <v>11.247999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B74" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C74" s="10">
+        <v>2.36</v>
+      </c>
+      <c r="D74" s="10">
+        <v>6.7530000000000001</v>
+      </c>
+      <c r="E74" s="10">
+        <v>0</v>
+      </c>
+      <c r="F74" s="10">
+        <v>0</v>
+      </c>
+      <c r="G74" s="10">
+        <v>0</v>
+      </c>
+      <c r="H74" s="10">
+        <v>0</v>
+      </c>
+      <c r="I74" s="10">
+        <v>0</v>
+      </c>
+      <c r="J74" s="10">
+        <f t="shared" si="4"/>
+        <v>9.1129999999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B75" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="16">
+        <v>2.758</v>
+      </c>
+      <c r="D75" s="16">
+        <v>1.4870000000000001</v>
+      </c>
+      <c r="E75" s="16">
+        <v>0</v>
+      </c>
+      <c r="F75" s="16">
+        <v>0</v>
+      </c>
+      <c r="G75" s="16">
+        <v>0</v>
+      </c>
+      <c r="H75" s="16">
+        <v>2.0382165605095541</v>
+      </c>
+      <c r="I75" s="16">
+        <v>0</v>
+      </c>
+      <c r="J75" s="16">
+        <f t="shared" si="4"/>
+        <v>8.3214331210191084</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B76" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="10">
+        <v>2.782</v>
+      </c>
+      <c r="D76" s="10">
+        <v>3.5110000000000001</v>
+      </c>
+      <c r="E76" s="10">
+        <v>0</v>
+      </c>
+      <c r="F76" s="10">
+        <v>0</v>
+      </c>
+      <c r="G76" s="10">
+        <v>0</v>
+      </c>
+      <c r="H76" s="10">
+        <v>0</v>
+      </c>
+      <c r="I76" s="10">
+        <v>0</v>
+      </c>
+      <c r="J76" s="10">
+        <f t="shared" si="4"/>
+        <v>6.2930000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B77" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="16">
+        <v>1.492</v>
+      </c>
+      <c r="D77" s="16">
+        <v>4.702</v>
+      </c>
+      <c r="E77" s="16">
+        <v>0</v>
+      </c>
+      <c r="F77" s="16">
+        <v>0</v>
+      </c>
+      <c r="G77" s="16">
+        <v>0</v>
+      </c>
+      <c r="H77" s="16">
+        <v>0</v>
+      </c>
+      <c r="I77" s="16">
+        <v>0</v>
+      </c>
+      <c r="J77" s="16">
+        <f t="shared" si="4"/>
+        <v>6.194</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" s="10">
+        <v>1.929</v>
+      </c>
+      <c r="D78" s="10">
+        <v>2.5449999999999999</v>
+      </c>
+      <c r="E78" s="10">
+        <v>0</v>
+      </c>
+      <c r="F78" s="10">
+        <v>0</v>
+      </c>
+      <c r="G78" s="10">
+        <v>0</v>
+      </c>
+      <c r="H78" s="10">
+        <v>0</v>
+      </c>
+      <c r="I78" s="10">
+        <v>0</v>
+      </c>
+      <c r="J78" s="10">
+        <f t="shared" si="4"/>
+        <v>4.4740000000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B79" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="16">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="D79" s="16">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="E79" s="16">
+        <v>0</v>
+      </c>
+      <c r="F79" s="16">
+        <v>0</v>
+      </c>
+      <c r="G79" s="16">
+        <v>0</v>
+      </c>
+      <c r="H79" s="16">
+        <v>0</v>
+      </c>
+      <c r="I79" s="16">
+        <v>0</v>
+      </c>
+      <c r="J79" s="16">
+        <f t="shared" si="4"/>
+        <v>1.627</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" s="10">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="D80" s="10">
+        <v>0.59</v>
+      </c>
+      <c r="E80" s="10">
+        <v>0</v>
+      </c>
+      <c r="F80" s="10">
+        <v>0</v>
+      </c>
+      <c r="G80" s="10">
+        <v>0</v>
+      </c>
+      <c r="H80" s="10">
+        <v>0</v>
+      </c>
+      <c r="I80" s="10">
+        <v>0</v>
+      </c>
+      <c r="J80" s="10">
+        <f t="shared" si="4"/>
+        <v>1.3620000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B81" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="16">
+        <v>0.153</v>
+      </c>
+      <c r="D81" s="16">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="E81" s="16">
+        <v>0</v>
+      </c>
+      <c r="F81" s="16">
+        <v>0</v>
+      </c>
+      <c r="G81" s="16">
+        <v>0</v>
+      </c>
+      <c r="H81" s="16">
+        <v>0</v>
+      </c>
+      <c r="I81" s="16">
+        <v>0</v>
+      </c>
+      <c r="J81" s="16">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B82" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" s="10">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="D82" s="10">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="E82" s="10">
+        <v>0</v>
+      </c>
+      <c r="F82" s="10">
+        <v>0</v>
+      </c>
+      <c r="G82" s="10">
+        <v>0</v>
+      </c>
+      <c r="H82" s="10">
+        <v>0</v>
+      </c>
+      <c r="I82" s="10">
+        <v>0</v>
+      </c>
+      <c r="J82" s="10">
+        <f t="shared" si="4"/>
+        <v>0.26800000000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B83" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="D83" s="16">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E83" s="16">
+        <v>0</v>
+      </c>
+      <c r="F83" s="16">
+        <v>0</v>
+      </c>
+      <c r="G83" s="16">
+        <v>0</v>
+      </c>
+      <c r="H83" s="16">
+        <v>0</v>
+      </c>
+      <c r="I83" s="16">
+        <v>0</v>
+      </c>
+      <c r="J83" s="16">
+        <f t="shared" si="4"/>
+        <v>0.16699999999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B84" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84" s="10">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="D84" s="10">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E84" s="10">
+        <v>0</v>
+      </c>
+      <c r="F84" s="10">
+        <v>0</v>
+      </c>
+      <c r="G84" s="10">
+        <v>0</v>
+      </c>
+      <c r="H84" s="10">
+        <v>0</v>
+      </c>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10">
+        <f t="shared" si="4"/>
+        <v>0.108</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="B3:J28">
     <sortCondition descending="1" ref="J3:J28"/>
   </sortState>
+  <mergeCells count="9">
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:AA13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AM9" sqref="AM9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="26" width="3.28515625" customWidth="1"/>
+    <col min="27" max="27" width="3.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y3" s="25"/>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="R4" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="S4" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T4" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="U4" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="X4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y4" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z4" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA4" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="U5" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y5" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z5" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA5" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="P8" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="R8" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="S8" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="T8" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="U8" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="V8" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="W8" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="X8" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y8" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z8" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA8" s="34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="L9" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="M9" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="O9" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q9" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="R9" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="S9" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="T9" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="U9" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="V9" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="W9" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="X9" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y9" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z9" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA9" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="N12" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="O12" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="P12" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q12" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="R12" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="S12" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="T12" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="U12" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="V12" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="W12" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="X12" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y12" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z12" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA12" s="35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="P13" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="R13" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="U13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="X13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y13" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z13" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA13" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>